<commit_message>
edit MSE_PSNR_result.xlsx for reading convenience
</commit_message>
<xml_diff>
--- a/MSE_PSNR_result.xlsx
+++ b/MSE_PSNR_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="20520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="mse_psnr" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="158">
   <si>
     <t>01_8bit_Biateral_3.bmp</t>
   </si>
@@ -461,6 +461,62 @@
   </si>
   <si>
     <t>PSNR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>using fiilter type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>param</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bilateral</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gaussian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>median</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APNN with function type 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APNN with function 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>original filename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01_8bit.bmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_8bit.bmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cameraman.bmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>house.bmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jetplane.bmp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -493,7 +549,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -501,12 +557,101 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -784,1567 +929,2438 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C142"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J136" sqref="J136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
         <v>141</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+    <row r="2" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="G4" s="5">
         <v>1.07267</v>
       </c>
-      <c r="C3">
+      <c r="H4" s="6">
         <v>45.3613</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="G5" s="5">
         <v>3.4312299999999998</v>
       </c>
-      <c r="C4">
+      <c r="H5" s="6">
         <v>40.311500000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="G6" s="5">
         <v>11.5459</v>
       </c>
-      <c r="C5">
+      <c r="H6" s="6">
         <v>35.041699999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="G7" s="5">
         <v>32.6997</v>
       </c>
-      <c r="C6">
+      <c r="H7" s="6">
         <v>30.520600000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="G8" s="5">
         <v>67.752799999999993</v>
       </c>
-      <c r="C7">
+      <c r="H8" s="6">
         <v>27.3568</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="G9" s="5">
         <v>169.85300000000001</v>
       </c>
-      <c r="C8">
+      <c r="H9" s="6">
         <v>23.365300000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="G10" s="5">
         <v>56.802700000000002</v>
       </c>
-      <c r="C9">
+      <c r="H10" s="6">
         <v>28.122299999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="G11" s="5">
         <v>167.36199999999999</v>
       </c>
-      <c r="C10">
+      <c r="H11" s="6">
         <v>23.429500000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="G12" s="5">
         <v>432.17200000000003</v>
       </c>
-      <c r="C11">
+      <c r="H12" s="6">
         <v>19.3095</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="G13" s="5">
         <v>22.206499999999998</v>
       </c>
-      <c r="C12">
+      <c r="H13" s="6">
         <v>32.2012</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="G14" s="5">
         <v>82.542599999999993</v>
       </c>
-      <c r="C13">
+      <c r="H14" s="6">
         <v>26.499199999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
+      <c r="G15" s="5">
         <v>278.06799999999998</v>
       </c>
-      <c r="C14">
+      <c r="H15" s="6">
         <v>21.224499999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15">
+      <c r="G16" s="5">
         <v>6.3511800000000003</v>
       </c>
-      <c r="C15">
+      <c r="H16" s="6">
         <v>37.637500000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B16">
+      <c r="G17" s="5">
         <v>3.2031200000000003E-2</v>
       </c>
-      <c r="C16">
+      <c r="H17" s="6">
         <v>60.610300000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B17">
+      <c r="G18" s="5">
         <v>3.2031200000000003E-2</v>
       </c>
-      <c r="C17">
+      <c r="H18" s="6">
         <v>60.610300000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B18">
+      <c r="G19" s="5">
         <v>3.2031200000000003E-2</v>
       </c>
-      <c r="C18">
+      <c r="H19" s="6">
         <v>60.610300000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B19">
+      <c r="G20" s="5">
         <v>6.3511800000000003</v>
       </c>
-      <c r="C19">
+      <c r="H20" s="6">
         <v>37.637500000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B20">
+      <c r="G21" s="5">
         <v>51.770200000000003</v>
       </c>
-      <c r="C20">
+      <c r="H21" s="6">
         <v>28.525200000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21">
+      <c r="G22" s="5">
         <v>113.33499999999999</v>
       </c>
-      <c r="C21">
+      <c r="H22" s="6">
         <v>25.122399999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B22">
+      <c r="G23" s="5">
         <v>148.87</v>
       </c>
-      <c r="C22">
+      <c r="H23" s="6">
         <v>23.937999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B23">
+      <c r="G24" s="5">
         <v>6.35318</v>
       </c>
-      <c r="C23">
+      <c r="H24" s="6">
         <v>37.636099999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B24">
+      <c r="G25" s="5">
         <v>3.2031200000000003E-2</v>
       </c>
-      <c r="C24">
+      <c r="H25" s="6">
         <v>60.610300000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B25">
+      <c r="G26" s="5">
         <v>3.2031200000000003E-2</v>
       </c>
-      <c r="C25">
+      <c r="H26" s="6">
         <v>60.610300000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B26">
+      <c r="G27" s="5">
         <v>3.2031200000000003E-2</v>
       </c>
-      <c r="C26">
+      <c r="H27" s="6">
         <v>60.610300000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B27">
+      <c r="G28" s="5">
         <v>6.35318</v>
       </c>
-      <c r="C27">
+      <c r="H28" s="6">
         <v>37.636099999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B28">
+      <c r="G29" s="5">
         <v>51.761600000000001</v>
       </c>
-      <c r="C28">
+      <c r="H29" s="6">
         <v>28.5259</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B29">
+      <c r="G30" s="5">
         <v>113.336</v>
       </c>
-      <c r="C29">
+      <c r="H30" s="6">
         <v>25.122299999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
+    <row r="31" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B30">
+      <c r="G31" s="8">
         <v>148.87</v>
       </c>
-      <c r="C30">
+      <c r="H31" s="9">
         <v>23.937999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
+    <row r="32" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B31">
+      <c r="G34" s="5">
         <v>0.51099499999999998</v>
       </c>
-      <c r="C31">
+      <c r="H34" s="6">
         <v>51.012500000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B32">
+      <c r="G35" s="5">
         <v>0</v>
       </c>
-      <c r="C32" t="s">
+      <c r="H35" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
+      <c r="G36" s="5">
         <v>0</v>
       </c>
-      <c r="C33" t="s">
+      <c r="H36" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="G37" s="5">
         <v>928.07</v>
       </c>
-      <c r="C34">
+      <c r="H37" s="6">
         <v>18.4209</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B35">
+      <c r="G38" s="5">
         <v>1473.01</v>
       </c>
-      <c r="C35">
+      <c r="H38" s="6">
         <v>16.4146</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="G39" s="5">
         <v>2654.54</v>
       </c>
-      <c r="C36">
+      <c r="H39" s="6">
         <v>13.8568</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
+      <c r="G40" s="5">
         <v>1591.24</v>
       </c>
-      <c r="C37">
+      <c r="H40" s="6">
         <v>16.0793</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A41" s="4"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B38">
+      <c r="G41" s="5">
         <v>2829.31</v>
       </c>
-      <c r="C38">
+      <c r="H41" s="6">
         <v>13.5799</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B39">
+      <c r="G42" s="5">
         <v>5091.32</v>
       </c>
-      <c r="C39">
+      <c r="H42" s="6">
         <v>11.0284</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B40">
+      <c r="G43" s="5">
         <v>410.69200000000001</v>
       </c>
-      <c r="C40">
+      <c r="H43" s="6">
         <v>21.961500000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B41">
+      <c r="G44" s="5">
         <v>1232.08</v>
       </c>
-      <c r="C41">
+      <c r="H44" s="6">
         <v>17.190300000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B42">
+      <c r="G45" s="5">
         <v>3285.54</v>
       </c>
-      <c r="C42">
+      <c r="H45" s="6">
         <v>12.9306</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B43">
+      <c r="G46" s="5">
         <v>175.66900000000001</v>
       </c>
-      <c r="C43">
+      <c r="H46" s="6">
         <v>25.649699999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
+      <c r="G47" s="5">
         <v>0.11926100000000001</v>
       </c>
-      <c r="C44">
+      <c r="H47" s="6">
         <v>57.331699999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B45">
+      <c r="G48" s="5">
         <v>0.11926100000000001</v>
       </c>
-      <c r="C45">
+      <c r="H48" s="6">
         <v>57.331699999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B46">
+      <c r="G49" s="5">
         <v>0.11926100000000001</v>
       </c>
-      <c r="C46">
+      <c r="H49" s="6">
         <v>57.331699999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B47">
+      <c r="G50" s="5">
         <v>175.66900000000001</v>
       </c>
-      <c r="C47">
+      <c r="H50" s="6">
         <v>25.649699999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B48">
+      <c r="G51" s="5">
         <v>1238.83</v>
       </c>
-      <c r="C48">
+      <c r="H51" s="6">
         <v>17.166599999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B49">
+      <c r="G52" s="5">
         <v>2091.7199999999998</v>
       </c>
-      <c r="C49">
+      <c r="H52" s="6">
         <v>14.8916</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A53" s="4"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
+      <c r="G53" s="5">
         <v>2519.7600000000002</v>
       </c>
-      <c r="C50">
+      <c r="H53" s="6">
         <v>14.0831</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B51">
+      <c r="G54" s="5">
         <v>175.839</v>
       </c>
-      <c r="C51">
+      <c r="H54" s="6">
         <v>25.645499999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A55" s="4"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B52">
+      <c r="G55" s="5">
         <v>0.11926100000000001</v>
       </c>
-      <c r="C52">
+      <c r="H55" s="6">
         <v>57.331699999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A53" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B53">
+      <c r="G56" s="5">
         <v>0.11926100000000001</v>
       </c>
-      <c r="C53">
+      <c r="H56" s="6">
         <v>57.331699999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B54">
+      <c r="G57" s="5">
         <v>0.11926100000000001</v>
       </c>
-      <c r="C54">
+      <c r="H57" s="6">
         <v>57.331699999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A55" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B55">
+      <c r="G58" s="5">
         <v>175.839</v>
       </c>
-      <c r="C55">
+      <c r="H58" s="6">
         <v>25.645499999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A59" s="4"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B56">
+      <c r="G59" s="5">
         <v>1238.8900000000001</v>
       </c>
-      <c r="C56">
+      <c r="H59" s="6">
         <v>17.1663</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A57" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B57">
+      <c r="G60" s="5">
         <v>2092.52</v>
       </c>
-      <c r="C57">
+      <c r="H60" s="6">
         <v>14.89</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
+    <row r="61" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="7"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B58">
+      <c r="G61" s="8">
         <v>2519.7600000000002</v>
       </c>
-      <c r="C58">
+      <c r="H61" s="9">
         <v>14.0831</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A59" t="s">
+    <row r="62" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A63" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="3"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A64" s="4"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B59">
+      <c r="G64" s="5">
         <v>0.84464600000000001</v>
       </c>
-      <c r="C59">
+      <c r="H64" s="6">
         <v>48.864100000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A60" t="s">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A65" s="4"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B60">
+      <c r="G65" s="5">
         <v>3.0835300000000001</v>
       </c>
-      <c r="C60">
+      <c r="H65" s="6">
         <v>43.240299999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A66" s="4"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B61">
+      <c r="G66" s="5">
         <v>13.4984</v>
       </c>
-      <c r="C61">
+      <c r="H66" s="6">
         <v>36.828000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A62" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A67" s="4"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B62">
+      <c r="G67" s="5">
         <v>11.3233</v>
       </c>
-      <c r="C62">
+      <c r="H67" s="6">
         <v>37.591099999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A63" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A68" s="4"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B63">
+      <c r="G68" s="5">
         <v>29.572700000000001</v>
       </c>
-      <c r="C63">
+      <c r="H68" s="6">
         <v>33.421900000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A64" t="s">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A69" s="4"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B64">
+      <c r="G69" s="5">
         <v>91.228499999999997</v>
       </c>
-      <c r="C64">
+      <c r="H69" s="6">
         <v>28.529499999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A65" t="s">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A70" s="4"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B65">
+      <c r="G70" s="5">
         <v>19.443000000000001</v>
       </c>
-      <c r="C65">
+      <c r="H70" s="6">
         <v>35.243200000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A66" t="s">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A71" s="4"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B66">
+      <c r="G71" s="5">
         <v>83.269099999999995</v>
       </c>
-      <c r="C66">
+      <c r="H71" s="6">
         <v>28.925999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A67" t="s">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A72" s="4"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B67">
+      <c r="G72" s="5">
         <v>240.22900000000001</v>
       </c>
-      <c r="C67">
+      <c r="H72" s="6">
         <v>24.3246</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A68" t="s">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A73" s="4"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B68">
+      <c r="G73" s="5">
         <v>13.086600000000001</v>
       </c>
-      <c r="C68">
+      <c r="H73" s="6">
         <v>36.962499999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A69" t="s">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A74" s="4"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B69">
+      <c r="G74" s="5">
         <v>48.160200000000003</v>
       </c>
-      <c r="C69">
+      <c r="H74" s="6">
         <v>31.303899999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A70" t="s">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A75" s="4"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B70">
+      <c r="G75" s="5">
         <v>185.29300000000001</v>
       </c>
-      <c r="C70">
+      <c r="H75" s="6">
         <v>25.452200000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A71" t="s">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A76" s="4"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B71">
+      <c r="G76" s="5">
         <v>2.2479499999999999</v>
       </c>
-      <c r="C71">
+      <c r="H76" s="6">
         <v>44.612900000000003</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A72" t="s">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A77" s="4"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B72">
+      <c r="G77" s="5">
         <v>5.4397600000000001E-3</v>
       </c>
-      <c r="C72">
+      <c r="H77" s="6">
         <v>70.775000000000006</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A73" t="s">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A78" s="4"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B73">
+      <c r="G78" s="5">
         <v>5.4397600000000001E-3</v>
       </c>
-      <c r="C73">
+      <c r="H78" s="6">
         <v>70.775000000000006</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A74" t="s">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A79" s="4"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B74">
+      <c r="G79" s="5">
         <v>5.4397600000000001E-3</v>
       </c>
-      <c r="C74">
+      <c r="H79" s="6">
         <v>70.775000000000006</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A75" t="s">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A80" s="4"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B75">
+      <c r="G80" s="5">
         <v>2.2479499999999999</v>
       </c>
-      <c r="C75">
+      <c r="H80" s="6">
         <v>44.612900000000003</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A76" t="s">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A81" s="4"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B76">
+      <c r="G81" s="5">
         <v>20.923200000000001</v>
       </c>
-      <c r="C76">
+      <c r="H81" s="6">
         <v>34.924500000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A77" t="s">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A82" s="4"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B77">
+      <c r="G82" s="5">
         <v>53.501600000000003</v>
       </c>
-      <c r="C77">
+      <c r="H82" s="6">
         <v>30.847100000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A78" t="s">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A83" s="4"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B78">
+      <c r="G83" s="5">
         <v>73.052099999999996</v>
       </c>
-      <c r="C78">
+      <c r="H83" s="6">
         <v>29.494499999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A79" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A84" s="4"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B79">
+      <c r="G84" s="5">
         <v>2.2477900000000002</v>
       </c>
-      <c r="C79">
+      <c r="H84" s="6">
         <v>44.613199999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A80" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A85" s="4"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B80">
+      <c r="G85" s="5">
         <v>5.4397600000000001E-3</v>
       </c>
-      <c r="C80">
+      <c r="H85" s="6">
         <v>70.775000000000006</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A81" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A86" s="4"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B81">
+      <c r="G86" s="5">
         <v>5.4397600000000001E-3</v>
       </c>
-      <c r="C81">
+      <c r="H86" s="6">
         <v>70.775000000000006</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A82" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A87" s="4"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B82">
+      <c r="G87" s="5">
         <v>5.4397600000000001E-3</v>
       </c>
-      <c r="C82">
+      <c r="H87" s="6">
         <v>70.775000000000006</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A83" t="s">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A88" s="4"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B83">
+      <c r="G88" s="5">
         <v>2.2477900000000002</v>
       </c>
-      <c r="C83">
+      <c r="H88" s="6">
         <v>44.613199999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A84" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A89" s="4"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B84">
+      <c r="G89" s="5">
         <v>20.923500000000001</v>
       </c>
-      <c r="C84">
+      <c r="H89" s="6">
         <v>34.924500000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A85" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A90" s="4"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B85">
+      <c r="G90" s="5">
         <v>53.507100000000001</v>
       </c>
-      <c r="C85">
+      <c r="H90" s="6">
         <v>30.846699999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A86" t="s">
+    <row r="91" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="7"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B86">
+      <c r="G91" s="8">
         <v>73.052099999999996</v>
       </c>
-      <c r="C86">
+      <c r="H91" s="9">
         <v>29.494499999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A87" t="s">
+    <row r="92" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A93" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="3"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A94" s="4"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B87">
+      <c r="G94" s="5">
         <v>0.52723699999999996</v>
       </c>
-      <c r="C87">
+      <c r="H94" s="6">
         <v>50.876600000000003</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A88" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A95" s="4"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B88">
+      <c r="G95" s="5">
         <v>1.6552</v>
       </c>
-      <c r="C88">
+      <c r="H95" s="6">
         <v>45.908200000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A89" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A96" s="4"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B89">
+      <c r="G96" s="5">
         <v>8.0330999999999992</v>
       </c>
-      <c r="C89">
+      <c r="H96" s="6">
         <v>39.047800000000002</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A90" t="s">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A97" s="4"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B90">
+      <c r="G97" s="5">
         <v>1.6903699999999999</v>
       </c>
-      <c r="C90">
+      <c r="H97" s="6">
         <v>45.816899999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A91" t="s">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A98" s="4"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B91">
+      <c r="G98" s="5">
         <v>4.8308400000000002</v>
       </c>
-      <c r="C91">
+      <c r="H98" s="6">
         <v>41.256500000000003</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A92" t="s">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A99" s="4"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B92">
+      <c r="G99" s="5">
         <v>21.654900000000001</v>
       </c>
-      <c r="C92">
+      <c r="H99" s="6">
         <v>34.741100000000003</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A93" t="s">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A100" s="4"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B93">
+      <c r="G100" s="5">
         <v>2.9025099999999999</v>
       </c>
-      <c r="C93">
+      <c r="H100" s="6">
         <v>43.468899999999998</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A94" t="s">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A101" s="4"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B94">
+      <c r="G101" s="5">
         <v>15.453900000000001</v>
       </c>
-      <c r="C94">
+      <c r="H101" s="6">
         <v>36.206299999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A95" t="s">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A102" s="4"/>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B95">
+      <c r="G102" s="5">
         <v>76.243899999999996</v>
       </c>
-      <c r="C95">
+      <c r="H102" s="6">
         <v>29.2746</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A96" t="s">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A103" s="4"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B96">
+      <c r="G103" s="5">
         <v>1.34002</v>
       </c>
-      <c r="C96">
+      <c r="H103" s="6">
         <v>46.825600000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A97" t="s">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A104" s="4"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B97">
+      <c r="G104" s="5">
         <v>6.8351199999999999</v>
       </c>
-      <c r="C97">
+      <c r="H104" s="6">
         <v>39.749200000000002</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A98" t="s">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A105" s="4"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B98">
+      <c r="G105" s="5">
         <v>35.970999999999997</v>
       </c>
-      <c r="C98">
+      <c r="H105" s="6">
         <v>32.537199999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A99" t="s">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A106" s="4"/>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B99">
+      <c r="G106" s="5">
         <v>0.38511299999999998</v>
       </c>
-      <c r="C99">
+      <c r="H106" s="6">
         <v>52.2408</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A100" t="s">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A107" s="4"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B100">
+      <c r="G107" s="5">
         <v>2.1675099999999999E-2</v>
       </c>
-      <c r="C100">
+      <c r="H107" s="6">
         <v>64.737099999999998</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A101" t="s">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A108" s="4"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B101">
+      <c r="G108" s="5">
         <v>2.1675099999999999E-2</v>
       </c>
-      <c r="C101">
+      <c r="H108" s="6">
         <v>64.737099999999998</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A102" t="s">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A109" s="4"/>
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B102">
+      <c r="G109" s="5">
         <v>2.1675099999999999E-2</v>
       </c>
-      <c r="C102">
+      <c r="H109" s="6">
         <v>64.737099999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A103" t="s">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A110" s="4"/>
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B103">
+      <c r="G110" s="5">
         <v>0.38511299999999998</v>
       </c>
-      <c r="C103">
+      <c r="H110" s="6">
         <v>52.2408</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A104" t="s">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A111" s="4"/>
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B104">
+      <c r="G111" s="5">
         <v>3.70017</v>
       </c>
-      <c r="C104">
+      <c r="H111" s="6">
         <v>42.414499999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A105" t="s">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A112" s="4"/>
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B105">
+      <c r="G112" s="5">
         <v>12.738</v>
       </c>
-      <c r="C105">
+      <c r="H112" s="6">
         <v>37.045699999999997</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A106" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A113" s="4"/>
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B106">
+      <c r="G113" s="5">
         <v>19.039899999999999</v>
       </c>
-      <c r="C106">
+      <c r="H113" s="6">
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A107" t="s">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A114" s="4"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B107">
+      <c r="G114" s="5">
         <v>0.38487199999999999</v>
       </c>
-      <c r="C107">
+      <c r="H114" s="6">
         <v>52.243499999999997</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A108" t="s">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A115" s="4"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B108">
+      <c r="G115" s="5">
         <v>2.1675099999999999E-2</v>
       </c>
-      <c r="C108">
+      <c r="H115" s="6">
         <v>64.737099999999998</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A109" t="s">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A116" s="4"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B109">
+      <c r="G116" s="5">
         <v>2.1675099999999999E-2</v>
       </c>
-      <c r="C109">
+      <c r="H116" s="6">
         <v>64.737099999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A110" t="s">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A117" s="4"/>
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B110">
+      <c r="G117" s="5">
         <v>2.1675099999999999E-2</v>
       </c>
-      <c r="C110">
+      <c r="H117" s="6">
         <v>64.737099999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A111" t="s">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A118" s="4"/>
+      <c r="B118" s="5"/>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B111">
+      <c r="G118" s="5">
         <v>0.38487199999999999</v>
       </c>
-      <c r="C111">
+      <c r="H118" s="6">
         <v>52.243499999999997</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A112" t="s">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A119" s="4"/>
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B112">
+      <c r="G119" s="5">
         <v>3.69977</v>
       </c>
-      <c r="C112">
+      <c r="H119" s="6">
         <v>42.414900000000003</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A113" t="s">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A120" s="4"/>
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="5"/>
+      <c r="F120" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B113">
+      <c r="G120" s="5">
         <v>12.7376</v>
       </c>
-      <c r="C113">
+      <c r="H120" s="6">
         <v>37.0458</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A114" t="s">
+    <row r="121" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="7"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B114">
+      <c r="G121" s="8">
         <v>19.039899999999999</v>
       </c>
-      <c r="C114">
+      <c r="H121" s="9">
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A115" t="s">
+    <row r="122" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="5"/>
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="5"/>
+      <c r="H122" s="5"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A123" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+      <c r="H123" s="3"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A124" s="4"/>
+      <c r="B124" s="5"/>
+      <c r="C124" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B115">
+      <c r="G124" s="5">
         <v>1.3897299999999999</v>
       </c>
-      <c r="C115">
+      <c r="H124" s="6">
         <v>45.8429</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A116" t="s">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A125" s="4"/>
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B116">
+      <c r="G125" s="5">
         <v>4.3509599999999997</v>
       </c>
-      <c r="C116">
+      <c r="H125" s="6">
         <v>40.886400000000002</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A117" t="s">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A126" s="4"/>
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B117">
+      <c r="G126" s="5">
         <v>14.5778</v>
       </c>
-      <c r="C117">
+      <c r="H126" s="6">
         <v>35.635300000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A118" t="s">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A127" s="4"/>
+      <c r="B127" s="5"/>
+      <c r="C127" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B118">
+      <c r="G127" s="5">
         <v>18.16</v>
       </c>
-      <c r="C118">
+      <c r="H127" s="6">
         <v>34.681100000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A119" t="s">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A128" s="4"/>
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B119">
+      <c r="G128" s="5">
         <v>40.040500000000002</v>
       </c>
-      <c r="C119">
+      <c r="H128" s="6">
         <v>31.247199999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A120" t="s">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A129" s="4"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B120">
+      <c r="G129" s="5">
         <v>103.914</v>
       </c>
-      <c r="C120">
+      <c r="H129" s="6">
         <v>27.105499999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A121" t="s">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A130" s="4"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B121">
+      <c r="G130" s="5">
         <v>30.38</v>
       </c>
-      <c r="C121">
+      <c r="H130" s="6">
         <v>32.446399999999997</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A122" t="s">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A131" s="4"/>
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B122">
+      <c r="G131" s="5">
         <v>98.8994</v>
       </c>
-      <c r="C122">
+      <c r="H131" s="6">
         <v>27.3203</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A123" t="s">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A132" s="4"/>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B123">
+      <c r="G132" s="5">
         <v>244.86600000000001</v>
       </c>
-      <c r="C123">
+      <c r="H132" s="6">
         <v>23.382999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A124" t="s">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A133" s="4"/>
+      <c r="B133" s="5"/>
+      <c r="C133" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B124">
+      <c r="G133" s="5">
         <v>19.2773</v>
       </c>
-      <c r="C124">
+      <c r="H133" s="6">
         <v>34.421799999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A125" t="s">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A134" s="4"/>
+      <c r="B134" s="5"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B125">
+      <c r="G134" s="5">
         <v>67.075199999999995</v>
       </c>
-      <c r="C125">
+      <c r="H134" s="6">
         <v>29.006599999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A126" t="s">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A135" s="4"/>
+      <c r="B135" s="5"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B126">
+      <c r="G135" s="5">
         <v>189.476</v>
       </c>
-      <c r="C126">
+      <c r="H135" s="6">
         <v>24.496700000000001</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A127" t="s">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A136" s="4"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D136" s="5"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B127">
+      <c r="G136" s="5">
         <v>3.7887599999999999</v>
       </c>
-      <c r="C127">
+      <c r="H136" s="6">
         <v>41.487299999999998</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A128" t="s">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A137" s="4"/>
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="5"/>
+      <c r="F137" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B128">
+      <c r="G137" s="5">
         <v>7.7579499999999996E-2</v>
       </c>
-      <c r="C128">
+      <c r="H137" s="6">
         <v>58.3748</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A129" t="s">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A138" s="4"/>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B129">
+      <c r="G138" s="5">
         <v>7.7579499999999996E-2</v>
       </c>
-      <c r="C129">
+      <c r="H138" s="6">
         <v>58.3748</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A130" t="s">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A139" s="4"/>
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B130">
+      <c r="G139" s="5">
         <v>7.7579499999999996E-2</v>
       </c>
-      <c r="C130">
+      <c r="H139" s="6">
         <v>58.3748</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A131" t="s">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A140" s="4"/>
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B131">
+      <c r="G140" s="5">
         <v>3.7887599999999999</v>
       </c>
-      <c r="C131">
+      <c r="H140" s="6">
         <v>41.487299999999998</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A132" t="s">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A141" s="4"/>
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="5"/>
+      <c r="F141" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B132">
+      <c r="G141" s="5">
         <v>29.457899999999999</v>
       </c>
-      <c r="C132">
+      <c r="H141" s="6">
         <v>32.580199999999998</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A133" t="s">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A142" s="4"/>
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="5"/>
+      <c r="F142" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B133">
+      <c r="G142" s="5">
         <v>64.941699999999997</v>
       </c>
-      <c r="C133">
+      <c r="H142" s="6">
         <v>29.146999999999998</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A134" t="s">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A143" s="4"/>
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="5"/>
+      <c r="F143" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B134">
+      <c r="G143" s="5">
         <v>85.013800000000003</v>
       </c>
-      <c r="C134">
+      <c r="H143" s="6">
         <v>27.9773</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A135" t="s">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A144" s="4"/>
+      <c r="B144" s="5"/>
+      <c r="C144" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D144" s="5"/>
+      <c r="E144" s="5"/>
+      <c r="F144" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B135">
+      <c r="G144" s="5">
         <v>3.7879299999999998</v>
       </c>
-      <c r="C135">
+      <c r="H144" s="6">
         <v>41.488199999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A136" t="s">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A145" s="4"/>
+      <c r="B145" s="5"/>
+      <c r="C145" s="5"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="5"/>
+      <c r="F145" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B136">
+      <c r="G145" s="5">
         <v>7.7579499999999996E-2</v>
       </c>
-      <c r="C136">
+      <c r="H145" s="6">
         <v>58.3748</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A137" t="s">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A146" s="4"/>
+      <c r="B146" s="5"/>
+      <c r="C146" s="5"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="5"/>
+      <c r="F146" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B137">
+      <c r="G146" s="5">
         <v>7.7579499999999996E-2</v>
       </c>
-      <c r="C137">
+      <c r="H146" s="6">
         <v>58.3748</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A138" t="s">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A147" s="4"/>
+      <c r="B147" s="5"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B138">
+      <c r="G147" s="5">
         <v>7.7579499999999996E-2</v>
       </c>
-      <c r="C138">
+      <c r="H147" s="6">
         <v>58.3748</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A139" t="s">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A148" s="4"/>
+      <c r="B148" s="5"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B139">
+      <c r="G148" s="5">
         <v>3.7879299999999998</v>
       </c>
-      <c r="C139">
+      <c r="H148" s="6">
         <v>41.488199999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A140" t="s">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A149" s="4"/>
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B140">
+      <c r="G149" s="5">
         <v>29.456099999999999</v>
       </c>
-      <c r="C140">
+      <c r="H149" s="6">
         <v>32.580500000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A141" t="s">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A150" s="4"/>
+      <c r="B150" s="5"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B141">
+      <c r="G150" s="5">
         <v>64.941299999999998</v>
       </c>
-      <c r="C141">
+      <c r="H150" s="6">
         <v>29.146999999999998</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A142" t="s">
+    <row r="151" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="7"/>
+      <c r="B151" s="8"/>
+      <c r="C151" s="8"/>
+      <c r="D151" s="8"/>
+      <c r="E151" s="8"/>
+      <c r="F151" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B142">
+      <c r="G151" s="8">
         <v>85.013800000000003</v>
       </c>
-      <c r="C142">
+      <c r="H151" s="9">
         <v>27.9773</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>